<commit_message>
feat: add export quantity
</commit_message>
<xml_diff>
--- a/exports/invoice_template.xlsx
+++ b/exports/invoice_template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dang.nguyenhai/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EA2859-DB3A-8440-B8CE-86066CFBA55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1425ED-B91C-004E-B6FB-8DBA28F49C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="16080" xr2:uid="{42B9C3C5-ADDF-2D47-A595-A92C02917BAE}"/>
+    <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="15800" xr2:uid="{42B9C3C5-ADDF-2D47-A595-A92C02917BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$40</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>グエン　カン　ズィ</t>
   </si>
@@ -228,13 +228,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t xml:space="preserve"> 年  　 月 　日 </t>
-    <rPh sb="9" eb="10">
-      <t>ニチ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>8.未成年の方からの商品の買取は（保護者の同意書がない限り）お断りしております。上記確認事項に同意しましたので、</t>
   </si>
   <si>
@@ -250,6 +243,12 @@
   <si>
     <t>状態</t>
     <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>順番</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 年  　 月 　日 </t>
   </si>
 </sst>
 </file>
@@ -432,7 +431,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -499,6 +498,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -525,9 +536,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -852,10 +860,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -863,180 +871,195 @@
     <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="23" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.6640625" style="1"/>
+    <col min="7" max="7" width="6.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="30">
-      <c r="B1" s="26" t="s">
+    <row r="1" spans="1:23" ht="30">
+      <c r="B1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-    </row>
-    <row r="2" spans="1:22" s="5" customFormat="1" ht="17" customHeight="1">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+    </row>
+    <row r="2" spans="1:23" s="5" customFormat="1" ht="17" customHeight="1">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-    </row>
-    <row r="3" spans="1:22" ht="21" customHeight="1">
-      <c r="B3" s="27" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+    </row>
+    <row r="3" spans="1:23" ht="21" customHeight="1">
+      <c r="B3" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="G3" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" spans="1:22" s="5" customFormat="1" ht="14" customHeight="1">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="G3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+    </row>
+    <row r="4" spans="1:23" s="5" customFormat="1" ht="14" customHeight="1">
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="G4" s="10"/>
       <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="1:22" ht="23" customHeight="1">
-      <c r="A5" s="28" t="s">
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:23" ht="23" customHeight="1">
+      <c r="A5" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="2" t="s">
+      <c r="F5" s="34"/>
+      <c r="G5" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:22" ht="22" customHeight="1">
-      <c r="A6" s="28" t="s">
+      <c r="H5" s="32"/>
+      <c r="I5" s="2"/>
+      <c r="K5" s="22"/>
+    </row>
+    <row r="6" spans="1:23" ht="22" customHeight="1">
+      <c r="A6" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="28"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="28" t="s">
+      <c r="F6" s="34"/>
+      <c r="G6" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="28"/>
-    </row>
-    <row r="7" spans="1:22" ht="20" customHeight="1">
-      <c r="A7" s="29" t="s">
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+    </row>
+    <row r="7" spans="1:23" ht="20" customHeight="1">
+      <c r="A7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="33" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="32" t="s">
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="32"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:22" ht="19" customHeight="1">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:22" s="5" customFormat="1" ht="19" customHeight="1">
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:23" ht="19" customHeight="1">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:23" s="5" customFormat="1" ht="19" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" spans="1:22" ht="21" customHeight="1">
+      <c r="I9" s="13"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:23" ht="21" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="24"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>32</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>23</v>
       </c>
       <c r="G10" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="23"/>
-    </row>
-    <row r="11" spans="1:22" ht="23" customHeight="1">
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="1:23" ht="23" customHeight="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="23"/>
-    </row>
-    <row r="12" spans="1:22" ht="23" customHeight="1">
+      <c r="G11" s="23"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="27"/>
+    </row>
+    <row r="12" spans="1:23" ht="23" customHeight="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="27"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="23"/>
-    </row>
-    <row r="14" spans="1:22" ht="20" customHeight="1">
+      <c r="G12" s="23"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="27"/>
+    </row>
+    <row r="14" spans="1:23" ht="20" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -1045,11 +1068,12 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:22" ht="20" customHeight="1">
+      <c r="I14" s="6"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:23" ht="20" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
@@ -1058,9 +1082,9 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="2"/>
+      <c r="I15" s="6"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -1074,19 +1098,20 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
-    </row>
-    <row r="16" spans="1:22" ht="19" customHeight="1">
-      <c r="A16" s="20" t="s">
+      <c r="W15" s="2"/>
+    </row>
+    <row r="16" spans="1:23" ht="19" customHeight="1">
+      <c r="A16" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="2"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -1100,19 +1125,20 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
-    </row>
-    <row r="17" spans="1:22" ht="20" customHeight="1">
-      <c r="A17" s="20" t="s">
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" spans="1:23" ht="20" customHeight="1">
+      <c r="A17" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="2"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1126,109 +1152,116 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-    </row>
-    <row r="18" spans="1:22" ht="17">
-      <c r="A18" s="20" t="s">
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" spans="1:23" ht="17">
+      <c r="A18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-    </row>
-    <row r="19" spans="1:22" ht="20" customHeight="1">
-      <c r="A19" s="20" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="1:23" ht="20" customHeight="1">
+      <c r="A19" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-    </row>
-    <row r="20" spans="1:22" ht="20" customHeight="1">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="1:23" ht="20" customHeight="1">
+      <c r="A20" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-    </row>
-    <row r="21" spans="1:22" ht="20" customHeight="1">
-      <c r="A21" s="20" t="s">
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+    </row>
+    <row r="21" spans="1:23" ht="20" customHeight="1">
+      <c r="A21" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-    </row>
-    <row r="22" spans="1:22">
-      <c r="A22" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" ht="19" customHeight="1">
+    </row>
+    <row r="23" spans="1:23" ht="19" customHeight="1">
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
     </row>
-    <row r="24" spans="1:22" ht="46" customHeight="1">
+    <row r="24" spans="1:23" ht="46" customHeight="1">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="23"/>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="F24" s="25"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="27"/>
+    </row>
+    <row r="25" spans="1:23">
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
       <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="B1:H1"/>
+  <mergeCells count="26">
+    <mergeCell ref="B1:I1"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="C7:F8"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G7:I8"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="A20:I20"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: update export feature
</commit_message>
<xml_diff>
--- a/exports/invoice_template.xlsx
+++ b/exports/invoice_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dang.nguyenhai/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1425ED-B91C-004E-B6FB-8DBA28F49C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA527F4-54E6-834E-957F-4F6C05D0D7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="15800" xr2:uid="{42B9C3C5-ADDF-2D47-A595-A92C02917BAE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>グエン　カン　ズィ</t>
   </si>
@@ -247,15 +247,12 @@
   <si>
     <t>順番</t>
   </si>
-  <si>
-    <t xml:space="preserve"> 年  　 月 　日 </t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -340,6 +337,13 @@
       <name val="Times New Roman"/>
       <family val="2"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -431,7 +435,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -537,10 +541,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -863,20 +870,20 @@
   <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" style="5" customWidth="1"/>
     <col min="8" max="8" width="6.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" style="1" customWidth="1"/>
     <col min="10" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
@@ -893,8 +900,8 @@
       <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:23" s="5" customFormat="1" ht="17" customHeight="1">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="32" t="s">
@@ -911,9 +918,7 @@
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
       <c r="E3" s="31"/>
-      <c r="G3" s="32" t="s">
-        <v>33</v>
-      </c>
+      <c r="G3" s="32"/>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
     </row>
@@ -973,29 +978,29 @@
         <v>5</v>
       </c>
       <c r="B7" s="33"/>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="35" t="s">
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:23" ht="19" customHeight="1">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:23" s="5" customFormat="1" ht="19" customHeight="1">
@@ -1235,7 +1240,7 @@
       <c r="I25" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="27">
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A5:B5"/>
@@ -1249,6 +1254,7 @@
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="A21:I21"/>
     <mergeCell ref="F24:I24"/>
     <mergeCell ref="H10:I10"/>

</xml_diff>